<commit_message>
Add calc numerator module
</commit_message>
<xml_diff>
--- a/NOAA_Test_Data_30_n.xlsx
+++ b/NOAA_Test_Data_30_n.xlsx
@@ -1,19 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E85D9B9A-2340-4FBF-A927-C5CEBECEDA59}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{E85D9B9A-2340-4FBF-A927-C5CEBECEDA59}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{BDD7C21F-FA46-4C49-9BF9-AE7DDCA86DB0}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -335,12 +343,12 @@
   <dimension ref="A1:C30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1590</v>
       </c>
@@ -351,7 +359,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2313</v>
       </c>
@@ -362,7 +370,7 @@
         <v>1952</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2804</v>
       </c>
@@ -373,7 +381,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3003</v>
       </c>
@@ -384,7 +392,7 @@
         <v>2428</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1468</v>
       </c>
@@ -395,7 +403,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1138</v>
       </c>
@@ -406,7 +414,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>994</v>
       </c>
@@ -417,7 +425,7 @@
         <v>747</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>433</v>
       </c>
@@ -428,7 +436,7 @@
         <v>857</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2416</v>
       </c>
@@ -439,7 +447,7 @@
         <v>1795</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1691</v>
       </c>
@@ -450,7 +458,7 @@
         <v>1785</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1037</v>
       </c>
@@ -461,7 +469,7 @@
         <v>785</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2571</v>
       </c>
@@ -472,7 +480,7 @@
         <v>1788</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1916</v>
       </c>
@@ -483,7 +491,7 @@
         <v>1798</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2447</v>
       </c>
@@ -494,7 +502,7 @@
         <v>1844</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>3054</v>
       </c>
@@ -505,7 +513,7 @@
         <v>1949</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>56</v>
       </c>
@@ -516,7 +524,7 @@
         <v>1788</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1416</v>
       </c>
@@ -527,7 +535,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2242</v>
       </c>
@@ -538,7 +546,7 @@
         <v>1634</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>614</v>
       </c>
@@ -549,7 +557,7 @@
         <v>871</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>494</v>
       </c>
@@ -560,7 +568,7 @@
         <v>1527</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>1404</v>
       </c>
@@ -571,7 +579,7 @@
         <v>897</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>1766</v>
       </c>
@@ -582,7 +590,7 @@
         <v>1652</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>732</v>
       </c>
@@ -593,7 +601,7 @@
         <v>846</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>1104</v>
       </c>
@@ -604,7 +612,7 @@
         <v>1490</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>452</v>
       </c>
@@ -615,7 +623,7 @@
         <v>886</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>2204</v>
       </c>
@@ -626,7 +634,7 @@
         <v>857</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>65</v>
       </c>
@@ -637,7 +645,7 @@
         <v>912</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>1940</v>
       </c>
@@ -648,7 +656,7 @@
         <v>874</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>45</v>
       </c>
@@ -659,7 +667,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>2573</v>
       </c>

</xml_diff>

<commit_message>
Have to multiply numerator by 4 for some reason?
</commit_message>
<xml_diff>
--- a/NOAA_Test_Data_30_n.xlsx
+++ b/NOAA_Test_Data_30_n.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{E85D9B9A-2340-4FBF-A927-C5CEBECEDA59}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{BDD7C21F-FA46-4C49-9BF9-AE7DDCA86DB0}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{E85D9B9A-2340-4FBF-A927-C5CEBECEDA59}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{37C3ACA9-A1B0-4B81-81B5-0EADA39B511D}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="555" yWindow="1215" windowWidth="4785" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -343,7 +343,7 @@
   <dimension ref="A1:C30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>